<commit_message>
bulk commit of seerstat rate files, all sites, first try, salivary only
</commit_message>
<xml_diff>
--- a/Results/SCC_SEER.xlsx
+++ b/Results/SCC_SEER.xlsx
@@ -373,10 +373,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +383,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,7 +668,8 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,51 +686,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="H2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="7" t="s">
         <v>93</v>
       </c>
     </row>
@@ -766,22 +769,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
-        <v>807</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="C7" s="5">
+        <v>807</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">

</xml_diff>

<commit_message>
added DB18 recoded IDCO without leuk lymph and skin, has counts only, updated to xlsx file with 99 or more counts highlighted. need to code individiual 48 ICD-O-3 recode sites by columns
</commit_message>
<xml_diff>
--- a/Results/SCC_SEER.xlsx
+++ b/Results/SCC_SEER.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7725" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$D$103</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="201">
   <si>
     <t>C000-C006,C008-C009</t>
   </si>
@@ -315,6 +319,318 @@
   </si>
   <si>
     <t>Table. Counts with these cancers histology squamous cell carcinoma/malignant behavior (behavior=3)</t>
+  </si>
+  <si>
+    <t>scc</t>
+  </si>
+  <si>
+    <t>non_scc</t>
+  </si>
+  <si>
+    <t>All Sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Oral Cavity and Pharynx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Tongue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Salivary Gland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Floor of Mouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Gum and Other Mouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nasopharynx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Tonsil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Oropharynx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Hypopharynx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Oral Cavity and Pharynx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Digestive System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Esophagus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Stomach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Small Intestine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Colon and Rectum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Colon excluding Rectum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Cecum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Appendix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Ascending Colon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Hepatic Flexure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Transverse Colon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Splenic Flexure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Descending Colon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Sigmoid Colon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Large Intestine, NOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Rectum and Rectosigmoid Junction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Rectosigmoid Junction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Rectum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Anus, Anal Canal and Anorectum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Liver and Intrahepatic Bile Duct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Liver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Intrahepatic Bile Duct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Gallbladder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Biliary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Pancreas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Retroperitoneum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Peritoneum, Omentum and Mesentery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Digestive Organs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Respiratory System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nose, Nasal Cavity and Middle Ear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Larynx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lung and Bronchus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Pleura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Trachea, Mediastinum and Other Respiratory Organs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bones and Joints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Soft Tissue including Heart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Skin excluding Basal and Squamous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Melanoma of the Skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Non-Epithelial Skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Breast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Female Genital System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Cervix Uteri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Corpus and Uterus, NOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Corpus Uteri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Uterus, NOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ovary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Vagina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Vulva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Female Genital Organs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Male Genital System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Prostate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Testis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Penis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Male Genital Organs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Urinary System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Urinary Bladder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Kidney and Renal Pelvis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ureter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Urinary Organs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Eye and Orbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Brain and Other Nervous System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Brain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Cranial Nerves Other Nervous System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Endocrine System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Thyroid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Endocrine including Thymus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Lymphoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Hodgkin Lymphoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Hodgkin - Nodal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Hodgkin - Extranodal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Non-Hodgkin Lymphoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      NHL - Nodal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      NHL - Extranodal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Myeloma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lymphocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Acute Lymphocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Chronic Lymphocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other Lymphocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Myeloid and Monocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Acute Myeloid Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Acute Monocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Chronic Myeloid Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other Myeloid/Monocytic Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Other Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Other Acute Leukemia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Aleukemic, Subleukemic and NOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mesothelioma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kaposi Sarcoma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Miscellaneous</t>
   </si>
 </sst>
 </file>
@@ -373,23 +689,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -667,9 +995,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,47 +1019,47 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>93</v>
       </c>
     </row>
@@ -769,22 +1097,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5">
-        <v>807</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="C7" s="4">
+        <v>807</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1245,4 +1573,1464 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="9">
+        <v>321257</v>
+      </c>
+      <c r="D2" s="9">
+        <v>4220710</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="9">
+        <v>84327</v>
+      </c>
+      <c r="D3" s="9">
+        <v>21613</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="9">
+        <v>6847</v>
+      </c>
+      <c r="D4">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="9">
+        <v>28033</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="9">
+        <v>2443</v>
+      </c>
+      <c r="D6" s="9">
+        <v>9568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="9">
+        <v>5651</v>
+      </c>
+      <c r="D7">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="9">
+        <v>10575</v>
+      </c>
+      <c r="D8" s="9">
+        <v>3670</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2563</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="9">
+        <v>17009</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3491</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="9">
+        <v>6015</v>
+      </c>
+      <c r="D12">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1700</v>
+      </c>
+      <c r="D13">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="9">
+        <v>29223</v>
+      </c>
+      <c r="D14" s="9">
+        <v>787138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="9">
+        <v>14179</v>
+      </c>
+      <c r="D15" s="9">
+        <v>30080</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16">
+        <v>554</v>
+      </c>
+      <c r="D16" s="9">
+        <v>67662</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17">
+        <v>18</v>
+      </c>
+      <c r="D17" s="9">
+        <v>18975</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1974</v>
+      </c>
+      <c r="D18" s="9">
+        <v>437899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19">
+        <v>92</v>
+      </c>
+      <c r="D19" s="9">
+        <v>314657</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" s="9">
+        <v>71730</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>6895</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9">
+        <v>57879</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="D23" s="9">
+        <v>15745</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9">
+        <v>27691</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" s="9">
+        <v>10436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="9">
+        <v>17907</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27" s="9">
+        <v>85939</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
+      <c r="D28" s="9">
+        <v>20435</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1882</v>
+      </c>
+      <c r="D29" s="9">
+        <v>123242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30">
+        <v>45</v>
+      </c>
+      <c r="D30" s="9">
+        <v>33775</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1837</v>
+      </c>
+      <c r="D31" s="9">
+        <v>89467</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="9">
+        <v>12124</v>
+      </c>
+      <c r="D32" s="9">
+        <v>5196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33">
+        <v>17</v>
+      </c>
+      <c r="D33" s="9">
+        <v>67548</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34" s="9">
+        <v>60899</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" s="9">
+        <v>6649</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36">
+        <v>138</v>
+      </c>
+      <c r="D36" s="9">
+        <v>10926</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+      <c r="D37" s="9">
+        <v>16537</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38">
+        <v>191</v>
+      </c>
+      <c r="D38" s="9">
+        <v>117298</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" s="9">
+        <v>3786</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9">
+        <v>6101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" s="9">
+        <v>5130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="9">
+        <v>148852</v>
+      </c>
+      <c r="D42" s="9">
+        <v>488054</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C43" s="9">
+        <v>3061</v>
+      </c>
+      <c r="D43" s="9">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>141</v>
+      </c>
+      <c r="C44" s="9">
+        <v>33108</v>
+      </c>
+      <c r="D44" s="9">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" s="9">
+        <v>112453</v>
+      </c>
+      <c r="D45" s="9">
+        <v>480121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47">
+        <v>230</v>
+      </c>
+      <c r="D47" s="9">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48">
+        <v>129</v>
+      </c>
+      <c r="D48" s="9">
+        <v>9211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49">
+        <v>193</v>
+      </c>
+      <c r="D49" s="9">
+        <v>31367</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>147</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50" s="9">
+        <v>217380</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51" s="9">
+        <v>200040</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" s="9">
+        <v>17340</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53">
+        <v>369</v>
+      </c>
+      <c r="D53" s="9">
+        <v>680946</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" s="9">
+        <v>40415</v>
+      </c>
+      <c r="D54" s="9">
+        <v>225160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>152</v>
+      </c>
+      <c r="C55" s="9">
+        <v>28026</v>
+      </c>
+      <c r="D55" s="9">
+        <v>14327</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56">
+        <v>485</v>
+      </c>
+      <c r="D56" s="9">
+        <v>132503</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57">
+        <v>429</v>
+      </c>
+      <c r="D57" s="9">
+        <v>128838</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C58">
+        <v>56</v>
+      </c>
+      <c r="D58" s="9">
+        <v>3665</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>156</v>
+      </c>
+      <c r="C59">
+        <v>217</v>
+      </c>
+      <c r="D59" s="9">
+        <v>69088</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="9">
+        <v>2346</v>
+      </c>
+      <c r="D60" s="9">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="9">
+        <v>9258</v>
+      </c>
+      <c r="D61" s="9">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>159</v>
+      </c>
+      <c r="C62">
+        <v>83</v>
+      </c>
+      <c r="D62" s="9">
+        <v>4397</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" s="9">
+        <v>3335</v>
+      </c>
+      <c r="D63" s="9">
+        <v>725306</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64">
+        <v>19</v>
+      </c>
+      <c r="D64" s="9">
+        <v>694655</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>162</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65" s="9">
+        <v>29325</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" s="9">
+        <v>3101</v>
+      </c>
+      <c r="D66">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67">
+        <v>213</v>
+      </c>
+      <c r="D67">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>165</v>
+      </c>
+      <c r="C68" s="9">
+        <v>3092</v>
+      </c>
+      <c r="D68" s="9">
+        <v>336209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>166</v>
+      </c>
+      <c r="C69" s="9">
+        <v>2410</v>
+      </c>
+      <c r="D69" s="9">
+        <v>190954</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>167</v>
+      </c>
+      <c r="C70">
+        <v>236</v>
+      </c>
+      <c r="D70" s="9">
+        <v>138804</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>168</v>
+      </c>
+      <c r="C71">
+        <v>66</v>
+      </c>
+      <c r="D71" s="9">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>169</v>
+      </c>
+      <c r="C72">
+        <v>380</v>
+      </c>
+      <c r="D72" s="9">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>170</v>
+      </c>
+      <c r="C73">
+        <v>835</v>
+      </c>
+      <c r="D73" s="9">
+        <v>7746</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" s="9">
+        <v>67354</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75" s="9">
+        <v>63113</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76" s="9">
+        <v>4241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77">
+        <v>239</v>
+      </c>
+      <c r="D77" s="9">
+        <v>115807</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78">
+        <v>99</v>
+      </c>
+      <c r="D78" s="9">
+        <v>108934</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79">
+        <v>140</v>
+      </c>
+      <c r="D79" s="9">
+        <v>6873</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80" s="9">
+        <v>218340</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>178</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" s="9">
+        <v>28646</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>179</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82" s="9">
+        <v>27907</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>180</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" s="9">
+        <v>189694</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" s="9">
+        <v>129314</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86" s="9">
+        <v>60380</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>184</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" s="9">
+        <v>60646</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>185</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" s="9">
+        <v>129091</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>186</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89" s="9">
+        <v>66943</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>187</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90" s="9">
+        <v>16710</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>188</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91" s="9">
+        <v>45990</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>189</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92" s="9">
+        <v>4243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93" s="9">
+        <v>55433</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94" s="9">
+        <v>35225</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>192</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95" s="9">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96" s="9">
+        <v>16194</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97" s="9">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98" s="9">
+        <v>6715</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>196</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99" s="9">
+        <v>2749</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>197</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100" s="9">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101" s="9">
+        <v>10086</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>199</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102" s="9">
+        <v>5966</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>200</v>
+      </c>
+      <c r="C103" s="9">
+        <v>10246</v>
+      </c>
+      <c r="D103" s="9">
+        <v>83290</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:D103"/>
+  <conditionalFormatting sqref="C2:C103">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>98</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>